<commit_message>
Added update to file
updated status of some of the proteins
</commit_message>
<xml_diff>
--- a/uniprot_validation_set.xlsx
+++ b/uniprot_validation_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpearson\Desktop\validation_project\VALIDATION SET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D6D7C4D-20B9-45D0-BAF9-A1F381B5102E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7DB42561-2A63-47C5-9E9D-F7A6468F2A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9153,23 +9153,23 @@
     <t>Only Ubiquitin like region: 705-788 IKVQVPNMQDKTEWKLNGQGLVFTLPLTDQVSVIKVKIHEATGMPAGKQKLQYEGIFIKDSNSLAYYNMASGAVIHLALKERGG</t>
   </si>
   <si>
-    <t>https://robetta.bakerlab.org/results.php?id=502205</t>
-  </si>
-  <si>
     <t xml:space="preserve">For Vkabat calculation used domains:  1: (1-25 undefined + 26-638 extracellular + 639-659 transmembrane), 2: (660-835 cytoplasmic) </t>
   </si>
   <si>
-    <t>ERROR ON SERVER</t>
-  </si>
-  <si>
     <t>For Vkabat calculation used domains: ???</t>
+  </si>
+  <si>
+    <t>Complete (not on GitHub)</t>
+  </si>
+  <si>
+    <t>https://robetta.bakerlab.org/results.php?id=502443</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9395,6 +9395,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9861,7 +9876,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -10039,45 +10054,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10152,9 +10128,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -10173,6 +10146,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10571,28 +10605,28 @@
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
-      <c r="K1" s="75" t="s">
+      <c r="K1" s="109" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="78" t="s">
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="112" t="s">
         <v>560</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="69" t="s">
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="103" t="s">
         <v>561</v>
       </c>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="71"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="104"/>
+      <c r="Z1" s="105"/>
       <c r="AC1" s="39" t="s">
         <v>2878</v>
       </c>
@@ -10608,16 +10642,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="38"/>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="107" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="72" t="s">
+      <c r="F2" s="106"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
       <c r="K2" s="8" t="s">
         <v>206</v>
       </c>
@@ -11856,7 +11890,7 @@
       <c r="D21" t="s">
         <v>104</v>
       </c>
-      <c r="H21" s="88" t="s">
+      <c r="H21" s="75" t="s">
         <v>3021</v>
       </c>
       <c r="I21" s="11" t="s">
@@ -14840,9 +14874,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091D803E-5FC9-4756-B9B7-361382611093}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B60" sqref="B60"/>
+      <selection pane="topRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14850,12 +14884,12 @@
     <col min="1" max="1" width="14.77734375" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.21875" style="62" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="52" customWidth="1"/>
-    <col min="4" max="4" width="63" style="116" customWidth="1"/>
-    <col min="5" max="5" width="39.77734375" style="52" customWidth="1"/>
-    <col min="6" max="6" width="33.77734375" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.44140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.5546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.33203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" style="102" customWidth="1"/>
+    <col min="5" max="5" width="55.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="58" customWidth="1"/>
+    <col min="8" max="9" width="23.77734375" style="63" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.21875" style="60" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" style="46" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.21875" style="46" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.77734375" style="46" bestFit="1" customWidth="1"/>
@@ -14914,7 +14948,7 @@
       <c r="C2" s="52">
         <v>296</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="97" t="s">
         <v>2934</v>
       </c>
       <c r="E2" s="53" t="s">
@@ -14948,11 +14982,11 @@
       <c r="A3" s="55" t="s">
         <v>569</v>
       </c>
-      <c r="B3" s="105"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="61">
         <v>385</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="97" t="s">
         <v>2935</v>
       </c>
       <c r="E3" s="53" t="s">
@@ -14982,14 +15016,14 @@
       <c r="M3" s="47"/>
       <c r="N3" s="47"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>570</v>
       </c>
       <c r="C4" s="52">
         <v>514</v>
       </c>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="97" t="s">
         <v>2936</v>
       </c>
       <c r="E4" s="53" t="s">
@@ -15019,14 +15053,14 @@
       <c r="M4" s="47"/>
       <c r="N4" s="47"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>2909</v>
       </c>
       <c r="C5" s="52">
         <v>630</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="97" t="s">
         <v>2937</v>
       </c>
       <c r="E5" s="53" t="s">
@@ -15056,14 +15090,14 @@
       <c r="M5" s="47"/>
       <c r="N5" s="47"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>572</v>
       </c>
       <c r="C6" s="52">
         <v>369</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="97" t="s">
         <v>2938</v>
       </c>
       <c r="E6" s="53" t="s">
@@ -15093,14 +15127,14 @@
       <c r="M6" s="47"/>
       <c r="N6" s="47"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
         <v>573</v>
       </c>
       <c r="C7" s="52">
         <v>541</v>
       </c>
-      <c r="D7" s="111" t="s">
+      <c r="D7" s="97" t="s">
         <v>2939</v>
       </c>
       <c r="E7" s="53" t="s">
@@ -15130,14 +15164,14 @@
       <c r="M7" s="47"/>
       <c r="N7" s="47"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
         <v>575</v>
       </c>
       <c r="C8" s="52">
         <v>148</v>
       </c>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="97" t="s">
         <v>2940</v>
       </c>
       <c r="E8" s="53" t="s">
@@ -15152,8 +15186,8 @@
       <c r="H8" s="63" t="s">
         <v>2988</v>
       </c>
-      <c r="I8" s="63" t="s">
-        <v>2988</v>
+      <c r="I8" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="J8" s="65" t="s">
         <v>2913</v>
@@ -15174,7 +15208,7 @@
       <c r="C9" s="52">
         <v>593</v>
       </c>
-      <c r="D9" s="111" t="s">
+      <c r="D9" s="97" t="s">
         <v>2941</v>
       </c>
       <c r="E9" s="53" t="s">
@@ -15211,7 +15245,7 @@
       <c r="C10" s="52">
         <v>537</v>
       </c>
-      <c r="D10" s="111" t="s">
+      <c r="D10" s="97" t="s">
         <v>2942</v>
       </c>
       <c r="E10" s="53" t="s">
@@ -15248,7 +15282,7 @@
       <c r="C11" s="52">
         <v>475</v>
       </c>
-      <c r="D11" s="111" t="s">
+      <c r="D11" s="97" t="s">
         <v>2943</v>
       </c>
       <c r="E11" s="53" t="s">
@@ -15278,14 +15312,14 @@
       <c r="M11" s="47"/>
       <c r="N11" s="47"/>
     </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
         <v>578</v>
       </c>
       <c r="C12" s="52">
         <v>461</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="97" t="s">
         <v>2944</v>
       </c>
       <c r="E12" s="53" t="s">
@@ -15315,15 +15349,15 @@
       <c r="M12" s="47"/>
       <c r="N12" s="47"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="55" t="s">
         <v>579</v>
       </c>
-      <c r="B13" s="105"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="61">
         <v>630</v>
       </c>
-      <c r="D13" s="112" t="s">
+      <c r="D13" s="98" t="s">
         <v>2945</v>
       </c>
       <c r="E13" s="53" t="s">
@@ -15357,11 +15391,11 @@
       <c r="A14" s="49" t="s">
         <v>580</v>
       </c>
-      <c r="B14" s="106"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="59">
         <v>354</v>
       </c>
-      <c r="D14" s="113" t="s">
+      <c r="D14" s="99" t="s">
         <v>2946</v>
       </c>
       <c r="E14" s="54" t="s">
@@ -15398,7 +15432,7 @@
       <c r="C15" s="52">
         <v>747</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="97" t="s">
         <v>2947</v>
       </c>
       <c r="E15" s="53" t="s">
@@ -15426,14 +15460,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="48" t="s">
         <v>2903</v>
       </c>
       <c r="C16" s="52">
         <v>173</v>
       </c>
-      <c r="D16" s="111" t="s">
+      <c r="D16" s="97" t="s">
         <v>2948</v>
       </c>
       <c r="E16" s="53" t="s">
@@ -15461,14 +15495,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
         <v>2895</v>
       </c>
       <c r="C17" s="52">
         <v>462</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="97" t="s">
         <v>2949</v>
       </c>
       <c r="E17" s="53" t="s">
@@ -15503,7 +15537,7 @@
       <c r="C18" s="52">
         <v>252</v>
       </c>
-      <c r="D18" s="111" t="s">
+      <c r="D18" s="97" t="s">
         <v>2950</v>
       </c>
       <c r="E18" s="53" t="s">
@@ -15531,39 +15565,39 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="95" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="89" t="s">
+    <row r="19" spans="1:12" s="82" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="76" t="s">
         <v>2898</v>
       </c>
-      <c r="B19" s="107"/>
-      <c r="C19" s="90">
+      <c r="B19" s="94"/>
+      <c r="C19" s="77">
         <v>1273</v>
       </c>
-      <c r="D19" s="114" t="s">
+      <c r="D19" s="100" t="s">
         <v>2951</v>
       </c>
-      <c r="E19" s="91" t="s">
+      <c r="E19" s="78" t="s">
         <v>2894</v>
       </c>
-      <c r="F19" s="92" t="s">
+      <c r="F19" s="79" t="s">
         <v>2889</v>
       </c>
-      <c r="G19" s="92" t="s">
+      <c r="G19" s="79" t="s">
         <v>2930</v>
       </c>
-      <c r="H19" s="93" t="s">
+      <c r="H19" s="80" t="s">
         <v>2988</v>
       </c>
-      <c r="I19" s="93" t="s">
+      <c r="I19" s="80" t="s">
         <v>2988</v>
       </c>
-      <c r="J19" s="94" t="s">
+      <c r="J19" s="81" t="s">
         <v>2924</v>
       </c>
-      <c r="K19" s="92" t="s">
+      <c r="K19" s="79" t="s">
         <v>2889</v>
       </c>
-      <c r="L19" s="92" t="s">
+      <c r="L19" s="79" t="s">
         <v>3020</v>
       </c>
     </row>
@@ -15574,7 +15608,7 @@
       <c r="C20" s="52">
         <v>75</v>
       </c>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="97" t="s">
         <v>2952</v>
       </c>
       <c r="E20" s="53" t="s">
@@ -15589,8 +15623,8 @@
       <c r="H20" s="63" t="s">
         <v>2988</v>
       </c>
-      <c r="I20" s="63" t="s">
-        <v>2988</v>
+      <c r="I20" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="J20" s="65" t="s">
         <v>2925</v>
@@ -15609,7 +15643,7 @@
       <c r="C21" s="52">
         <v>222</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="97" t="s">
         <v>2953</v>
       </c>
       <c r="E21" s="53" t="s">
@@ -15644,7 +15678,7 @@
       <c r="C22" s="52">
         <v>419</v>
       </c>
-      <c r="D22" s="111" t="s">
+      <c r="D22" s="97" t="s">
         <v>2954</v>
       </c>
       <c r="E22" s="53" t="s">
@@ -15672,14 +15706,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>2897</v>
       </c>
       <c r="C23" s="52">
         <v>641</v>
       </c>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="97" t="s">
         <v>2955</v>
       </c>
       <c r="E23" s="53" t="s">
@@ -15707,15 +15741,15 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="51" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
         <v>2905</v>
       </c>
-      <c r="B24" s="106"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="59">
         <v>732</v>
       </c>
-      <c r="D24" s="113" t="s">
+      <c r="D24" s="99" t="s">
         <v>2956</v>
       </c>
       <c r="E24" s="54" t="s">
@@ -15743,14 +15777,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="48" t="s">
         <v>585</v>
       </c>
       <c r="C25" s="52">
         <v>232</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="97" t="s">
         <v>2957</v>
       </c>
       <c r="E25" s="53" t="s">
@@ -15778,14 +15812,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>586</v>
       </c>
       <c r="C26" s="52">
         <v>231</v>
       </c>
-      <c r="D26" s="111" t="s">
+      <c r="D26" s="97" t="s">
         <v>2958</v>
       </c>
       <c r="E26" s="53" t="s">
@@ -15813,14 +15847,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="48" t="s">
         <v>587</v>
       </c>
       <c r="C27" s="52">
         <v>398</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="97" t="s">
         <v>2959</v>
       </c>
       <c r="E27" s="53" t="s">
@@ -15848,14 +15882,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
         <v>588</v>
       </c>
       <c r="C28" s="52">
         <v>405</v>
       </c>
-      <c r="D28" s="111" t="s">
+      <c r="D28" s="97" t="s">
         <v>2960</v>
       </c>
       <c r="E28" s="53" t="s">
@@ -15883,14 +15917,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="48" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="52">
         <v>149</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="97" t="s">
         <v>2961</v>
       </c>
       <c r="E29" s="53" t="s">
@@ -15902,8 +15936,8 @@
       <c r="G29" s="56" t="s">
         <v>2889</v>
       </c>
-      <c r="H29" s="63" t="s">
-        <v>2988</v>
+      <c r="H29" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="I29" s="63" t="s">
         <v>2988</v>
@@ -15918,14 +15952,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="48" t="s">
         <v>590</v>
       </c>
       <c r="C30" s="52">
         <v>376</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="97" t="s">
         <v>2962</v>
       </c>
       <c r="E30" s="53" t="s">
@@ -15953,14 +15987,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="48" t="s">
         <v>591</v>
       </c>
       <c r="C31" s="52">
         <v>127</v>
       </c>
-      <c r="D31" s="111" t="s">
+      <c r="D31" s="97" t="s">
         <v>2963</v>
       </c>
       <c r="E31" s="53" t="s">
@@ -15988,14 +16022,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="48" t="s">
         <v>592</v>
       </c>
       <c r="C32" s="52">
         <v>558</v>
       </c>
-      <c r="D32" s="111" t="s">
+      <c r="D32" s="97" t="s">
         <v>2964</v>
       </c>
       <c r="E32" s="53" t="s">
@@ -16023,14 +16057,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="48" t="s">
         <v>593</v>
       </c>
       <c r="C33" s="52">
         <v>448</v>
       </c>
-      <c r="D33" s="111" t="s">
+      <c r="D33" s="97" t="s">
         <v>2965</v>
       </c>
       <c r="E33" s="53" t="s">
@@ -16058,14 +16092,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="48" t="s">
         <v>594</v>
       </c>
       <c r="C34" s="52">
         <v>237</v>
       </c>
-      <c r="D34" s="111" t="s">
+      <c r="D34" s="97" t="s">
         <v>2966</v>
       </c>
       <c r="E34" s="53" t="s">
@@ -16100,7 +16134,7 @@
       <c r="C35" s="52">
         <v>325</v>
       </c>
-      <c r="D35" s="111" t="s">
+      <c r="D35" s="97" t="s">
         <v>2967</v>
       </c>
       <c r="E35" s="53" t="s">
@@ -16128,53 +16162,53 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="103" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="96" t="s">
+    <row r="36" spans="1:12" s="90" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="B36" s="108" t="s">
-        <v>3025</v>
-      </c>
-      <c r="C36" s="98">
+      <c r="B36" s="95" t="s">
+        <v>3024</v>
+      </c>
+      <c r="C36" s="85">
         <v>835</v>
       </c>
-      <c r="D36" s="115" t="s">
+      <c r="D36" s="101" t="s">
         <v>2968</v>
       </c>
-      <c r="E36" s="99" t="s">
+      <c r="E36" s="86" t="s">
         <v>2932</v>
       </c>
-      <c r="F36" s="87" t="s">
+      <c r="F36" s="74" t="s">
         <v>2889</v>
       </c>
-      <c r="G36" s="97" t="s">
+      <c r="G36" s="84" t="s">
         <v>2989</v>
       </c>
-      <c r="H36" s="104" t="s">
+      <c r="H36" s="91" t="s">
         <v>2988</v>
       </c>
-      <c r="I36" s="104" t="s">
+      <c r="I36" s="91" t="s">
         <v>2988</v>
       </c>
-      <c r="J36" s="101" t="s">
+      <c r="J36" s="88" t="s">
         <v>3001</v>
       </c>
-      <c r="K36" s="87" t="s">
+      <c r="K36" s="74" t="s">
         <v>2889</v>
       </c>
-      <c r="L36" s="87" t="s">
+      <c r="L36" s="74" t="s">
         <v>2889</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
         <v>598</v>
       </c>
-      <c r="B37" s="109"/>
+      <c r="B37" s="96"/>
       <c r="C37" s="52">
         <v>148</v>
       </c>
-      <c r="D37" s="111" t="s">
+      <c r="D37" s="97" t="s">
         <v>2969</v>
       </c>
       <c r="E37" s="53" t="s">
@@ -16202,41 +16236,41 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="103" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="96" t="s">
+    <row r="38" spans="1:12" s="123" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="83" t="s">
         <v>596</v>
       </c>
-      <c r="B38" s="110" t="s">
+      <c r="B38" s="117" t="s">
         <v>3023</v>
       </c>
-      <c r="C38" s="98">
+      <c r="C38" s="118">
         <v>84</v>
       </c>
-      <c r="D38" s="115" t="s">
+      <c r="D38" s="119" t="s">
         <v>2970</v>
       </c>
-      <c r="E38" s="99" t="s">
+      <c r="E38" s="120" t="s">
         <v>2932</v>
       </c>
-      <c r="F38" s="87" t="s">
+      <c r="F38" s="89" t="s">
         <v>2889</v>
       </c>
-      <c r="G38" s="87" t="s">
+      <c r="G38" s="89" t="s">
         <v>2889</v>
       </c>
-      <c r="H38" s="104" t="s">
+      <c r="H38" s="121" t="s">
         <v>2988</v>
       </c>
-      <c r="I38" s="104" t="s">
+      <c r="I38" s="121" t="s">
         <v>2988</v>
       </c>
-      <c r="J38" s="101" t="s">
-        <v>3024</v>
-      </c>
-      <c r="K38" s="97" t="s">
-        <v>3026</v>
-      </c>
-      <c r="L38" s="87" t="s">
+      <c r="J38" s="122" t="s">
+        <v>3027</v>
+      </c>
+      <c r="K38" s="89" t="s">
+        <v>2889</v>
+      </c>
+      <c r="L38" s="89" t="s">
         <v>2889</v>
       </c>
     </row>
@@ -16247,7 +16281,7 @@
       <c r="C39" s="52">
         <v>221</v>
       </c>
-      <c r="D39" s="111" t="s">
+      <c r="D39" s="97" t="s">
         <v>2971</v>
       </c>
       <c r="E39" s="53" t="s">
@@ -16275,15 +16309,15 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="51" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="49" t="s">
         <v>600</v>
       </c>
-      <c r="B40" s="106"/>
+      <c r="B40" s="93"/>
       <c r="C40" s="59">
         <v>207</v>
       </c>
-      <c r="D40" s="113" t="s">
+      <c r="D40" s="99" t="s">
         <v>2972</v>
       </c>
       <c r="E40" s="54" t="s">
@@ -16318,7 +16352,7 @@
       <c r="C41" s="52">
         <v>87</v>
       </c>
-      <c r="D41" s="111" t="s">
+      <c r="D41" s="97" t="s">
         <v>2973</v>
       </c>
       <c r="E41" s="53" t="s">
@@ -16346,14 +16380,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="48" t="s">
         <v>125</v>
       </c>
       <c r="C42" s="52">
         <v>135</v>
       </c>
-      <c r="D42" s="111" t="s">
+      <c r="D42" s="97" t="s">
         <v>2974</v>
       </c>
       <c r="E42" s="53" t="s">
@@ -16365,8 +16399,8 @@
       <c r="G42" s="56" t="s">
         <v>2889</v>
       </c>
-      <c r="H42" s="63" t="s">
-        <v>2988</v>
+      <c r="H42" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="I42" s="63" t="s">
         <v>2988</v>
@@ -16381,14 +16415,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="48" t="s">
         <v>101</v>
       </c>
       <c r="C43" s="52">
         <v>523</v>
       </c>
-      <c r="D43" s="111" t="s">
+      <c r="D43" s="97" t="s">
         <v>2975</v>
       </c>
       <c r="E43" s="53" t="s">
@@ -16416,14 +16450,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="48" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="52">
         <v>758</v>
       </c>
-      <c r="D44" s="111" t="s">
+      <c r="D44" s="97" t="s">
         <v>2976</v>
       </c>
       <c r="E44" s="53" t="s">
@@ -16451,14 +16485,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="48" t="s">
         <v>102</v>
       </c>
       <c r="C45" s="52">
         <v>213</v>
       </c>
-      <c r="D45" s="111" t="s">
+      <c r="D45" s="97" t="s">
         <v>2977</v>
       </c>
       <c r="E45" s="53" t="s">
@@ -16470,8 +16504,8 @@
       <c r="G45" s="56" t="s">
         <v>2889</v>
       </c>
-      <c r="H45" s="63" t="s">
-        <v>2988</v>
+      <c r="H45" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="I45" s="63" t="s">
         <v>2988</v>
@@ -16486,14 +16520,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="48" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="52">
         <v>112</v>
       </c>
-      <c r="D46" s="111" t="s">
+      <c r="D46" s="97" t="s">
         <v>2978</v>
       </c>
       <c r="E46" s="53" t="s">
@@ -16505,8 +16539,8 @@
       <c r="G46" s="56" t="s">
         <v>2889</v>
       </c>
-      <c r="H46" s="63" t="s">
-        <v>2988</v>
+      <c r="H46" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="I46" s="63" t="s">
         <v>2988</v>
@@ -16521,14 +16555,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="48" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="52">
         <v>256</v>
       </c>
-      <c r="D47" s="111" t="s">
+      <c r="D47" s="97" t="s">
         <v>2979</v>
       </c>
       <c r="E47" s="53" t="s">
@@ -16540,8 +16574,8 @@
       <c r="G47" s="56" t="s">
         <v>2889</v>
       </c>
-      <c r="H47" s="63" t="s">
-        <v>2988</v>
+      <c r="H47" s="116" t="s">
+        <v>3026</v>
       </c>
       <c r="I47" s="63" t="s">
         <v>2988</v>
@@ -16556,41 +16590,41 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="103" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="96" t="s">
+    <row r="48" spans="1:12" s="90" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="108" t="s">
-        <v>3027</v>
-      </c>
-      <c r="C48" s="98">
+      <c r="B48" s="95" t="s">
+        <v>3025</v>
+      </c>
+      <c r="C48" s="85">
         <v>773</v>
       </c>
-      <c r="D48" s="115" t="s">
+      <c r="D48" s="101" t="s">
         <v>2980</v>
       </c>
-      <c r="E48" s="99" t="s">
+      <c r="E48" s="86" t="s">
         <v>2933</v>
       </c>
-      <c r="F48" s="87" t="s">
+      <c r="F48" s="74" t="s">
         <v>2889</v>
       </c>
-      <c r="G48" s="97" t="s">
+      <c r="G48" s="84" t="s">
         <v>2989</v>
       </c>
-      <c r="H48" s="100" t="s">
+      <c r="H48" s="87" t="s">
         <v>2988</v>
       </c>
-      <c r="I48" s="100" t="s">
+      <c r="I48" s="87" t="s">
         <v>2988</v>
       </c>
-      <c r="J48" s="101" t="s">
+      <c r="J48" s="88" t="s">
         <v>3012</v>
       </c>
-      <c r="K48" s="102" t="s">
+      <c r="K48" s="89" t="s">
         <v>2889</v>
       </c>
-      <c r="L48" s="102" t="s">
+      <c r="L48" s="89" t="s">
         <v>2889</v>
       </c>
     </row>
@@ -16601,7 +16635,7 @@
       <c r="C49" s="52">
         <v>80</v>
       </c>
-      <c r="D49" s="111" t="s">
+      <c r="D49" s="97" t="s">
         <v>2981</v>
       </c>
       <c r="E49" s="53" t="s">
@@ -16629,14 +16663,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="48" t="s">
         <v>148</v>
       </c>
       <c r="C50" s="52">
         <v>526</v>
       </c>
-      <c r="D50" s="111" t="s">
+      <c r="D50" s="97" t="s">
         <v>2982</v>
       </c>
       <c r="E50" s="53" t="s">
@@ -16671,7 +16705,7 @@
       <c r="C51" s="52">
         <v>736</v>
       </c>
-      <c r="D51" s="111" t="s">
+      <c r="D51" s="97" t="s">
         <v>2983</v>
       </c>
       <c r="E51" s="53" t="s">
@@ -16699,14 +16733,14 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
         <v>128</v>
       </c>
       <c r="C52" s="52">
         <v>252</v>
       </c>
-      <c r="D52" s="111" t="s">
+      <c r="D52" s="97" t="s">
         <v>2984</v>
       </c>
       <c r="E52" s="53" t="s">
@@ -16741,7 +16775,7 @@
       <c r="C53" s="52">
         <v>279</v>
       </c>
-      <c r="D53" s="111" t="s">
+      <c r="D53" s="97" t="s">
         <v>2985</v>
       </c>
       <c r="E53" s="53" t="s">
@@ -16776,7 +16810,7 @@
       <c r="C54" s="52">
         <v>313</v>
       </c>
-      <c r="D54" s="111" t="s">
+      <c r="D54" s="97" t="s">
         <v>2986</v>
       </c>
       <c r="E54" s="53" t="s">
@@ -16811,7 +16845,7 @@
       <c r="C55" s="52">
         <v>146</v>
       </c>
-      <c r="D55" s="111" t="s">
+      <c r="D55" s="97" t="s">
         <v>2987</v>
       </c>
       <c r="E55" s="53" t="s">
@@ -16921,10 +16955,9 @@
     <hyperlink ref="J53" r:id="rId51" xr:uid="{A984C7AE-0A39-442D-9B74-0F643E39C3A8}"/>
     <hyperlink ref="J54" r:id="rId52" xr:uid="{1011A2DA-84B8-4DFB-8649-FEA531D12FA1}"/>
     <hyperlink ref="J55" r:id="rId53" xr:uid="{20C4EC70-96DA-42FE-BC83-586D80876C51}"/>
-    <hyperlink ref="J38" r:id="rId54" xr:uid="{60C7BE42-4E9E-47C8-BA64-48878F80E6F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId55"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -16949,16 +16982,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="115" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -17610,29 +17643,29 @@
         <v>723</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="84" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="82" t="s">
+    <row r="27" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="69" t="s">
         <v>724</v>
       </c>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="70" t="s">
         <v>725</v>
       </c>
-      <c r="C27" s="84" t="s">
-        <v>659</v>
-      </c>
-      <c r="D27" s="84" t="s">
+      <c r="C27" s="71" t="s">
+        <v>659</v>
+      </c>
+      <c r="D27" s="71" t="s">
         <v>726</v>
       </c>
-      <c r="E27" s="84" t="s">
+      <c r="E27" s="71" t="s">
         <v>727</v>
       </c>
-      <c r="F27" s="84" t="s">
+      <c r="F27" s="71" t="s">
         <v>728</v>
       </c>
-      <c r="G27" s="84" t="s">
+      <c r="G27" s="71" t="s">
         <v>669</v>
       </c>
-      <c r="H27" s="84" t="s">
+      <c r="H27" s="71" t="s">
         <v>729</v>
       </c>
     </row>
@@ -17662,29 +17695,29 @@
         <v>734</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="85" t="s">
+    <row r="29" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="72" t="s">
         <v>735</v>
       </c>
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="72" t="s">
         <v>736</v>
       </c>
-      <c r="C29" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D29" s="85" t="s">
+      <c r="C29" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D29" s="72" t="s">
         <v>737</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="E29" s="72" t="s">
         <v>738</v>
       </c>
-      <c r="F29" s="85" t="s">
+      <c r="F29" s="72" t="s">
         <v>739</v>
       </c>
-      <c r="G29" s="85" t="s">
+      <c r="G29" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H29" s="85" t="s">
+      <c r="H29" s="72" t="s">
         <v>740</v>
       </c>
     </row>
@@ -17740,29 +17773,29 @@
         <v>754</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="85" t="s">
+    <row r="32" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="B32" s="85" t="s">
+      <c r="B32" s="72" t="s">
         <v>755</v>
       </c>
-      <c r="C32" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D32" s="85" t="s">
+      <c r="C32" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D32" s="72" t="s">
         <v>756</v>
       </c>
-      <c r="E32" s="85" t="s">
+      <c r="E32" s="72" t="s">
         <v>757</v>
       </c>
-      <c r="F32" s="85" t="s">
+      <c r="F32" s="72" t="s">
         <v>758</v>
       </c>
-      <c r="G32" s="85" t="s">
+      <c r="G32" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H32" s="85" t="s">
+      <c r="H32" s="72" t="s">
         <v>759</v>
       </c>
     </row>
@@ -17792,29 +17825,29 @@
         <v>766</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="85" t="s">
+    <row r="34" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="72" t="s">
         <v>760</v>
       </c>
-      <c r="B34" s="85" t="s">
+      <c r="B34" s="72" t="s">
         <v>767</v>
       </c>
-      <c r="C34" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D34" s="85" t="s">
+      <c r="C34" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D34" s="72" t="s">
         <v>768</v>
       </c>
-      <c r="E34" s="85" t="s">
+      <c r="E34" s="72" t="s">
         <v>769</v>
       </c>
-      <c r="F34" s="85" t="s">
+      <c r="F34" s="72" t="s">
         <v>770</v>
       </c>
-      <c r="G34" s="85" t="s">
+      <c r="G34" s="72" t="s">
         <v>765</v>
       </c>
-      <c r="H34" s="85" t="s">
+      <c r="H34" s="72" t="s">
         <v>771</v>
       </c>
     </row>
@@ -17844,55 +17877,55 @@
         <v>777</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85" t="s">
+    <row r="36" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="72" t="s">
         <v>778</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="72" t="s">
         <v>779</v>
       </c>
-      <c r="C36" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D36" s="85" t="s">
+      <c r="C36" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D36" s="72" t="s">
         <v>780</v>
       </c>
-      <c r="E36" s="85" t="s">
+      <c r="E36" s="72" t="s">
         <v>781</v>
       </c>
-      <c r="F36" s="85" t="s">
+      <c r="F36" s="72" t="s">
         <v>782</v>
       </c>
-      <c r="G36" s="85" t="s">
+      <c r="G36" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H36" s="85" t="s">
+      <c r="H36" s="72" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="85" t="s">
+    <row r="37" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="72" t="s">
         <v>784</v>
       </c>
-      <c r="B37" s="85" t="s">
+      <c r="B37" s="72" t="s">
         <v>779</v>
       </c>
-      <c r="C37" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D37" s="85" t="s">
+      <c r="C37" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D37" s="72" t="s">
         <v>780</v>
       </c>
-      <c r="E37" s="85" t="s">
+      <c r="E37" s="72" t="s">
         <v>781</v>
       </c>
-      <c r="F37" s="85" t="s">
+      <c r="F37" s="72" t="s">
         <v>782</v>
       </c>
-      <c r="G37" s="85" t="s">
+      <c r="G37" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H37" s="85" t="s">
+      <c r="H37" s="72" t="s">
         <v>783</v>
       </c>
     </row>
@@ -17922,29 +17955,29 @@
         <v>790</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="85" t="s">
+    <row r="39" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="72" t="s">
         <v>791</v>
       </c>
-      <c r="B39" s="85" t="s">
+      <c r="B39" s="72" t="s">
         <v>792</v>
       </c>
-      <c r="C39" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D39" s="85" t="s">
+      <c r="C39" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D39" s="72" t="s">
         <v>793</v>
       </c>
-      <c r="E39" s="85" t="s">
+      <c r="E39" s="72" t="s">
         <v>794</v>
       </c>
-      <c r="F39" s="85" t="s">
+      <c r="F39" s="72" t="s">
         <v>795</v>
       </c>
-      <c r="G39" s="85" t="s">
+      <c r="G39" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H39" s="85" t="s">
+      <c r="H39" s="72" t="s">
         <v>796</v>
       </c>
     </row>
@@ -18078,29 +18111,29 @@
         <v>747</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="85" t="s">
+    <row r="45" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="72" t="s">
         <v>823</v>
       </c>
-      <c r="B45" s="85" t="s">
+      <c r="B45" s="72" t="s">
         <v>824</v>
       </c>
-      <c r="C45" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D45" s="85" t="s">
+      <c r="C45" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D45" s="72" t="s">
         <v>825</v>
       </c>
-      <c r="E45" s="85" t="s">
+      <c r="E45" s="72" t="s">
         <v>826</v>
       </c>
-      <c r="F45" s="85" t="s">
+      <c r="F45" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="G45" s="85" t="s">
+      <c r="G45" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H45" s="85" t="s">
+      <c r="H45" s="72" t="s">
         <v>828</v>
       </c>
     </row>
@@ -18130,29 +18163,29 @@
         <v>835</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="85" t="s">
+    <row r="47" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="72" t="s">
         <v>836</v>
       </c>
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="72" t="s">
         <v>736</v>
       </c>
-      <c r="C47" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D47" s="85" t="s">
+      <c r="C47" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D47" s="72" t="s">
         <v>737</v>
       </c>
-      <c r="E47" s="85" t="s">
+      <c r="E47" s="72" t="s">
         <v>738</v>
       </c>
-      <c r="F47" s="85" t="s">
+      <c r="F47" s="72" t="s">
         <v>739</v>
       </c>
-      <c r="G47" s="85" t="s">
+      <c r="G47" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H47" s="85" t="s">
+      <c r="H47" s="72" t="s">
         <v>740</v>
       </c>
     </row>
@@ -18364,29 +18397,29 @@
         <v>878</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="85" t="s">
+    <row r="56" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="72" t="s">
         <v>879</v>
       </c>
-      <c r="B56" s="85" t="s">
+      <c r="B56" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="C56" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D56" s="85" t="s">
+      <c r="C56" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D56" s="72" t="s">
         <v>881</v>
       </c>
-      <c r="E56" s="85" t="s">
+      <c r="E56" s="72" t="s">
         <v>882</v>
       </c>
-      <c r="F56" s="85" t="s">
+      <c r="F56" s="72" t="s">
         <v>883</v>
       </c>
-      <c r="G56" s="85" t="s">
+      <c r="G56" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H56" s="85" t="s">
+      <c r="H56" s="72" t="s">
         <v>884</v>
       </c>
     </row>
@@ -18780,29 +18813,29 @@
         <v>809</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="85" t="s">
+    <row r="72" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="72" t="s">
         <v>973</v>
       </c>
-      <c r="B72" s="85" t="s">
+      <c r="B72" s="72" t="s">
         <v>974</v>
       </c>
-      <c r="C72" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D72" s="85" t="s">
+      <c r="C72" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D72" s="72" t="s">
         <v>975</v>
       </c>
-      <c r="E72" s="85" t="s">
+      <c r="E72" s="72" t="s">
         <v>976</v>
       </c>
-      <c r="F72" s="85" t="s">
+      <c r="F72" s="72" t="s">
         <v>977</v>
       </c>
-      <c r="G72" s="85" t="s">
+      <c r="G72" s="72" t="s">
         <v>834</v>
       </c>
-      <c r="H72" s="85" t="s">
+      <c r="H72" s="72" t="s">
         <v>978</v>
       </c>
     </row>
@@ -18936,29 +18969,29 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="85" t="s">
+    <row r="78" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="72" t="s">
         <v>1009</v>
       </c>
-      <c r="B78" s="85" t="s">
+      <c r="B78" s="72" t="s">
         <v>1010</v>
       </c>
-      <c r="C78" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D78" s="85" t="s">
+      <c r="C78" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D78" s="72" t="s">
         <v>1011</v>
       </c>
-      <c r="E78" s="85" t="s">
+      <c r="E78" s="72" t="s">
         <v>1012</v>
       </c>
-      <c r="F78" s="85" t="s">
+      <c r="F78" s="72" t="s">
         <v>1013</v>
       </c>
-      <c r="G78" s="85" t="s">
+      <c r="G78" s="72" t="s">
         <v>717</v>
       </c>
-      <c r="H78" s="85" t="s">
+      <c r="H78" s="72" t="s">
         <v>1014</v>
       </c>
     </row>
@@ -19222,29 +19255,29 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="85" t="s">
+    <row r="89" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="72" t="s">
         <v>1073</v>
       </c>
-      <c r="B89" s="85" t="s">
+      <c r="B89" s="72" t="s">
         <v>1074</v>
       </c>
-      <c r="C89" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D89" s="85" t="s">
+      <c r="C89" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D89" s="72" t="s">
         <v>1075</v>
       </c>
-      <c r="E89" s="85" t="s">
+      <c r="E89" s="72" t="s">
         <v>1076</v>
       </c>
-      <c r="F89" s="85" t="s">
+      <c r="F89" s="72" t="s">
         <v>1077</v>
       </c>
-      <c r="G89" s="85" t="s">
+      <c r="G89" s="72" t="s">
         <v>746</v>
       </c>
-      <c r="H89" s="85" t="s">
+      <c r="H89" s="72" t="s">
         <v>1078</v>
       </c>
     </row>
@@ -19300,29 +19333,29 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="85" t="s">
+    <row r="92" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="72" t="s">
         <v>1090</v>
       </c>
-      <c r="B92" s="85" t="s">
+      <c r="B92" s="72" t="s">
         <v>1091</v>
       </c>
-      <c r="C92" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D92" s="85" t="s">
+      <c r="C92" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D92" s="72" t="s">
         <v>1092</v>
       </c>
-      <c r="E92" s="85" t="s">
+      <c r="E92" s="72" t="s">
         <v>1093</v>
       </c>
-      <c r="F92" s="85" t="s">
+      <c r="F92" s="72" t="s">
         <v>1094</v>
       </c>
-      <c r="G92" s="85" t="s">
+      <c r="G92" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H92" s="85" t="s">
+      <c r="H92" s="72" t="s">
         <v>1095</v>
       </c>
     </row>
@@ -19404,29 +19437,29 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="85" t="s">
+    <row r="96" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="72" t="s">
         <v>1115</v>
       </c>
-      <c r="B96" s="85" t="s">
+      <c r="B96" s="72" t="s">
         <v>1116</v>
       </c>
-      <c r="C96" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D96" s="85" t="s">
+      <c r="C96" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D96" s="72" t="s">
         <v>1117</v>
       </c>
-      <c r="E96" s="85" t="s">
+      <c r="E96" s="72" t="s">
         <v>1118</v>
       </c>
-      <c r="F96" s="85" t="s">
+      <c r="F96" s="72" t="s">
         <v>1119</v>
       </c>
-      <c r="G96" s="85" t="s">
+      <c r="G96" s="72" t="s">
         <v>1120</v>
       </c>
-      <c r="H96" s="85" t="s">
+      <c r="H96" s="72" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -19456,29 +19489,29 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="85" t="s">
+    <row r="98" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="72" t="s">
         <v>1122</v>
       </c>
-      <c r="B98" s="85" t="s">
+      <c r="B98" s="72" t="s">
         <v>1128</v>
       </c>
-      <c r="C98" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D98" s="85" t="s">
+      <c r="C98" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D98" s="72" t="s">
         <v>1129</v>
       </c>
-      <c r="E98" s="85" t="s">
+      <c r="E98" s="72" t="s">
         <v>1130</v>
       </c>
-      <c r="F98" s="85" t="s">
+      <c r="F98" s="72" t="s">
         <v>1131</v>
       </c>
-      <c r="G98" s="85" t="s">
+      <c r="G98" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H98" s="85" t="s">
+      <c r="H98" s="72" t="s">
         <v>1132</v>
       </c>
     </row>
@@ -19534,81 +19567,81 @@
         <v>873</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="85" t="s">
+    <row r="101" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="72" t="s">
         <v>1140</v>
       </c>
-      <c r="B101" s="85" t="s">
+      <c r="B101" s="72" t="s">
         <v>1145</v>
       </c>
-      <c r="C101" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D101" s="85" t="s">
+      <c r="C101" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D101" s="72" t="s">
         <v>1146</v>
       </c>
-      <c r="E101" s="85" t="s">
+      <c r="E101" s="72" t="s">
         <v>1147</v>
       </c>
-      <c r="F101" s="85" t="s">
+      <c r="F101" s="72" t="s">
         <v>1148</v>
       </c>
-      <c r="G101" s="85" t="s">
+      <c r="G101" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H101" s="85" t="s">
+      <c r="H101" s="72" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="85" t="s">
+    <row r="102" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="72" t="s">
         <v>1150</v>
       </c>
-      <c r="B102" s="85" t="s">
+      <c r="B102" s="72" t="s">
         <v>1151</v>
       </c>
-      <c r="C102" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D102" s="85" t="s">
+      <c r="C102" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D102" s="72" t="s">
         <v>1152</v>
       </c>
-      <c r="E102" s="85" t="s">
+      <c r="E102" s="72" t="s">
         <v>1153</v>
       </c>
-      <c r="F102" s="85" t="s">
+      <c r="F102" s="72" t="s">
         <v>1154</v>
       </c>
-      <c r="G102" s="85" t="s">
+      <c r="G102" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H102" s="85" t="s">
+      <c r="H102" s="72" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="85" t="s">
+    <row r="103" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="72" t="s">
         <v>1156</v>
       </c>
-      <c r="B103" s="85" t="s">
+      <c r="B103" s="72" t="s">
         <v>1157</v>
       </c>
-      <c r="C103" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D103" s="85" t="s">
+      <c r="C103" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D103" s="72" t="s">
         <v>1158</v>
       </c>
-      <c r="E103" s="85" t="s">
+      <c r="E103" s="72" t="s">
         <v>1159</v>
       </c>
-      <c r="F103" s="85" t="s">
+      <c r="F103" s="72" t="s">
         <v>1160</v>
       </c>
-      <c r="G103" s="85" t="s">
+      <c r="G103" s="72" t="s">
         <v>1161</v>
       </c>
-      <c r="H103" s="85" t="s">
+      <c r="H103" s="72" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -19664,55 +19697,55 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="85" t="s">
+    <row r="106" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="72" t="s">
         <v>1173</v>
       </c>
-      <c r="B106" s="85" t="s">
+      <c r="B106" s="72" t="s">
         <v>1174</v>
       </c>
-      <c r="C106" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D106" s="85" t="s">
+      <c r="C106" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D106" s="72" t="s">
         <v>1175</v>
       </c>
-      <c r="E106" s="85" t="s">
+      <c r="E106" s="72" t="s">
         <v>1176</v>
       </c>
-      <c r="F106" s="85" t="s">
+      <c r="F106" s="72" t="s">
         <v>1177</v>
       </c>
-      <c r="G106" s="85" t="s">
+      <c r="G106" s="72" t="s">
         <v>746</v>
       </c>
-      <c r="H106" s="85" t="s">
+      <c r="H106" s="72" t="s">
         <v>1178</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="85" t="s">
+    <row r="107" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="72" t="s">
         <v>1179</v>
       </c>
-      <c r="B107" s="85" t="s">
+      <c r="B107" s="72" t="s">
         <v>1180</v>
       </c>
-      <c r="C107" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D107" s="85" t="s">
+      <c r="C107" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D107" s="72" t="s">
         <v>1181</v>
       </c>
-      <c r="E107" s="85" t="s">
+      <c r="E107" s="72" t="s">
         <v>1182</v>
       </c>
-      <c r="F107" s="85" t="s">
+      <c r="F107" s="72" t="s">
         <v>1183</v>
       </c>
-      <c r="G107" s="85" t="s">
+      <c r="G107" s="72" t="s">
         <v>765</v>
       </c>
-      <c r="H107" s="85" t="s">
+      <c r="H107" s="72" t="s">
         <v>1184</v>
       </c>
     </row>
@@ -19742,29 +19775,29 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="85" t="s">
+    <row r="109" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="72" t="s">
         <v>1191</v>
       </c>
-      <c r="B109" s="85" t="s">
+      <c r="B109" s="72" t="s">
         <v>1192</v>
       </c>
-      <c r="C109" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D109" s="85" t="s">
+      <c r="C109" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D109" s="72" t="s">
         <v>1193</v>
       </c>
-      <c r="E109" s="85" t="s">
+      <c r="E109" s="72" t="s">
         <v>1194</v>
       </c>
-      <c r="F109" s="85" t="s">
+      <c r="F109" s="72" t="s">
         <v>1195</v>
       </c>
-      <c r="G109" s="85" t="s">
+      <c r="G109" s="72" t="s">
         <v>834</v>
       </c>
-      <c r="H109" s="85" t="s">
+      <c r="H109" s="72" t="s">
         <v>1196</v>
       </c>
     </row>
@@ -19820,29 +19853,29 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="85" t="s">
+    <row r="112" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="72" t="s">
         <v>1203</v>
       </c>
-      <c r="B112" s="85" t="s">
+      <c r="B112" s="72" t="s">
         <v>597</v>
       </c>
-      <c r="C112" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D112" s="85" t="s">
+      <c r="C112" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D112" s="72" t="s">
         <v>1209</v>
       </c>
-      <c r="E112" s="85" t="s">
+      <c r="E112" s="72" t="s">
         <v>1210</v>
       </c>
-      <c r="F112" s="85" t="s">
+      <c r="F112" s="72" t="s">
         <v>1211</v>
       </c>
-      <c r="G112" s="85" t="s">
+      <c r="G112" s="72" t="s">
         <v>746</v>
       </c>
-      <c r="H112" s="85" t="s">
+      <c r="H112" s="72" t="s">
         <v>1212</v>
       </c>
     </row>
@@ -19872,29 +19905,29 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="85" t="s">
+    <row r="114" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="72" t="s">
         <v>1220</v>
       </c>
-      <c r="B114" s="85" t="s">
+      <c r="B114" s="72" t="s">
         <v>1221</v>
       </c>
-      <c r="C114" s="85" t="s">
+      <c r="C114" s="72" t="s">
         <v>652</v>
       </c>
-      <c r="D114" s="85" t="s">
+      <c r="D114" s="72" t="s">
         <v>1222</v>
       </c>
-      <c r="E114" s="85" t="s">
+      <c r="E114" s="72" t="s">
         <v>1223</v>
       </c>
-      <c r="F114" s="85" t="s">
+      <c r="F114" s="72" t="s">
         <v>1224</v>
       </c>
-      <c r="G114" s="85" t="s">
+      <c r="G114" s="72" t="s">
         <v>1225</v>
       </c>
-      <c r="H114" s="85" t="s">
+      <c r="H114" s="72" t="s">
         <v>1226</v>
       </c>
     </row>
@@ -19976,55 +20009,55 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="85" t="s">
+    <row r="118" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="72" t="s">
         <v>1244</v>
       </c>
-      <c r="B118" s="85" t="s">
+      <c r="B118" s="72" t="s">
         <v>1245</v>
       </c>
-      <c r="C118" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D118" s="85" t="s">
+      <c r="C118" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D118" s="72" t="s">
         <v>1246</v>
       </c>
-      <c r="E118" s="85" t="s">
+      <c r="E118" s="72" t="s">
         <v>1247</v>
       </c>
-      <c r="F118" s="85" t="s">
+      <c r="F118" s="72" t="s">
         <v>1248</v>
       </c>
-      <c r="G118" s="85" t="s">
+      <c r="G118" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H118" s="85" t="s">
+      <c r="H118" s="72" t="s">
         <v>1249</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="85" t="s">
+    <row r="119" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="72" t="s">
         <v>1250</v>
       </c>
-      <c r="B119" s="85" t="s">
+      <c r="B119" s="72" t="s">
         <v>1251</v>
       </c>
-      <c r="C119" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D119" s="85" t="s">
+      <c r="C119" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D119" s="72" t="s">
         <v>1252</v>
       </c>
-      <c r="E119" s="85" t="s">
+      <c r="E119" s="72" t="s">
         <v>1253</v>
       </c>
-      <c r="F119" s="85" t="s">
+      <c r="F119" s="72" t="s">
         <v>1254</v>
       </c>
-      <c r="G119" s="85" t="s">
+      <c r="G119" s="72" t="s">
         <v>1255</v>
       </c>
-      <c r="H119" s="85" t="s">
+      <c r="H119" s="72" t="s">
         <v>1256</v>
       </c>
     </row>
@@ -20158,29 +20191,29 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="85" t="s">
+    <row r="125" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="72" t="s">
         <v>1286</v>
       </c>
-      <c r="B125" s="85" t="s">
+      <c r="B125" s="72" t="s">
         <v>1287</v>
       </c>
-      <c r="C125" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D125" s="85" t="s">
+      <c r="C125" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D125" s="72" t="s">
         <v>1288</v>
       </c>
-      <c r="E125" s="85" t="s">
+      <c r="E125" s="72" t="s">
         <v>1289</v>
       </c>
-      <c r="F125" s="85" t="s">
+      <c r="F125" s="72" t="s">
         <v>1290</v>
       </c>
-      <c r="G125" s="85" t="s">
+      <c r="G125" s="72" t="s">
         <v>746</v>
       </c>
-      <c r="H125" s="85" t="s">
+      <c r="H125" s="72" t="s">
         <v>1291</v>
       </c>
     </row>
@@ -20366,55 +20399,55 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="133" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="85" t="s">
+    <row r="133" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="72" t="s">
         <v>1324</v>
       </c>
-      <c r="B133" s="85" t="s">
+      <c r="B133" s="72" t="s">
         <v>1325</v>
       </c>
-      <c r="C133" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D133" s="85" t="s">
+      <c r="C133" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D133" s="72" t="s">
         <v>1326</v>
       </c>
-      <c r="E133" s="85" t="s">
+      <c r="E133" s="72" t="s">
         <v>1289</v>
       </c>
-      <c r="F133" s="85" t="s">
+      <c r="F133" s="72" t="s">
         <v>1327</v>
       </c>
-      <c r="G133" s="85" t="s">
+      <c r="G133" s="72" t="s">
         <v>1328</v>
       </c>
-      <c r="H133" s="85" t="s">
+      <c r="H133" s="72" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="85" t="s">
+    <row r="134" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="72" t="s">
         <v>1330</v>
       </c>
-      <c r="B134" s="85" t="s">
+      <c r="B134" s="72" t="s">
         <v>1331</v>
       </c>
-      <c r="C134" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D134" s="85" t="s">
+      <c r="C134" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D134" s="72" t="s">
         <v>1332</v>
       </c>
-      <c r="E134" s="85" t="s">
+      <c r="E134" s="72" t="s">
         <v>1333</v>
       </c>
-      <c r="F134" s="85" t="s">
+      <c r="F134" s="72" t="s">
         <v>1334</v>
       </c>
-      <c r="G134" s="85" t="s">
+      <c r="G134" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H134" s="85" t="s">
+      <c r="H134" s="72" t="s">
         <v>1335</v>
       </c>
     </row>
@@ -20496,29 +20529,29 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="85" t="s">
+    <row r="138" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="72" t="s">
         <v>1356</v>
       </c>
-      <c r="B138" s="85" t="s">
+      <c r="B138" s="72" t="s">
         <v>1357</v>
       </c>
-      <c r="C138" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D138" s="85" t="s">
+      <c r="C138" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D138" s="72" t="s">
         <v>1358</v>
       </c>
-      <c r="E138" s="85" t="s">
+      <c r="E138" s="72" t="s">
         <v>1359</v>
       </c>
-      <c r="F138" s="85" t="s">
+      <c r="F138" s="72" t="s">
         <v>1360</v>
       </c>
-      <c r="G138" s="85" t="s">
+      <c r="G138" s="72" t="s">
         <v>669</v>
       </c>
-      <c r="H138" s="85" t="s">
+      <c r="H138" s="72" t="s">
         <v>1361</v>
       </c>
     </row>
@@ -20574,29 +20607,29 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="85" t="s">
+    <row r="141" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="72" t="s">
         <v>1373</v>
       </c>
-      <c r="B141" s="85" t="s">
+      <c r="B141" s="72" t="s">
         <v>1374</v>
       </c>
-      <c r="C141" s="85" t="s">
+      <c r="C141" s="72" t="s">
         <v>652</v>
       </c>
-      <c r="D141" s="85" t="s">
+      <c r="D141" s="72" t="s">
         <v>1375</v>
       </c>
-      <c r="E141" s="85" t="s">
+      <c r="E141" s="72" t="s">
         <v>1376</v>
       </c>
-      <c r="F141" s="85" t="s">
+      <c r="F141" s="72" t="s">
         <v>1377</v>
       </c>
-      <c r="G141" s="85" t="s">
+      <c r="G141" s="72" t="s">
         <v>1378</v>
       </c>
-      <c r="H141" s="85" t="s">
+      <c r="H141" s="72" t="s">
         <v>1379</v>
       </c>
     </row>
@@ -20626,29 +20659,29 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="86" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="86" t="s">
+    <row r="143" spans="1:8" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="73" t="s">
         <v>1380</v>
       </c>
-      <c r="B143" s="86" t="s">
+      <c r="B143" s="73" t="s">
         <v>1386</v>
       </c>
-      <c r="C143" s="86" t="s">
-        <v>659</v>
-      </c>
-      <c r="D143" s="86" t="s">
+      <c r="C143" s="73" t="s">
+        <v>659</v>
+      </c>
+      <c r="D143" s="73" t="s">
         <v>1387</v>
       </c>
-      <c r="E143" s="86" t="s">
+      <c r="E143" s="73" t="s">
         <v>1388</v>
       </c>
-      <c r="F143" s="86" t="s">
+      <c r="F143" s="73" t="s">
         <v>1389</v>
       </c>
-      <c r="G143" s="86" t="s">
+      <c r="G143" s="73" t="s">
         <v>1071</v>
       </c>
-      <c r="H143" s="86" t="s">
+      <c r="H143" s="73" t="s">
         <v>1335</v>
       </c>
     </row>
@@ -20912,29 +20945,29 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="85" t="s">
+    <row r="154" spans="1:8" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="72" t="s">
         <v>1446</v>
       </c>
-      <c r="B154" s="85" t="s">
+      <c r="B154" s="72" t="s">
         <v>1447</v>
       </c>
-      <c r="C154" s="85" t="s">
-        <v>659</v>
-      </c>
-      <c r="D154" s="85" t="s">
+      <c r="C154" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="D154" s="72" t="s">
         <v>1448</v>
       </c>
-      <c r="E154" s="85" t="s">
+      <c r="E154" s="72" t="s">
         <v>1449</v>
       </c>
-      <c r="F154" s="85" t="s">
+      <c r="F154" s="72" t="s">
         <v>1450</v>
       </c>
-      <c r="G154" s="85" t="s">
+      <c r="G154" s="72" t="s">
         <v>1451</v>
       </c>
-      <c r="H154" s="85" t="s">
+      <c r="H154" s="72" t="s">
         <v>1452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated status of jobs
</commit_message>
<xml_diff>
--- a/uniprot_validation_set.xlsx
+++ b/uniprot_validation_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpearson\Desktop\validation_project\VALIDATION SET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DB1BAFFB-B699-4187-9C92-77FF7F81E9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4B6C7D61-DBF2-4636-BF66-6BD37DEB60B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uniprot" sheetId="1" r:id="rId1"/>
@@ -9165,9 +9165,6 @@
     <t>https://robetta.bakerlab.org/results.php?id=502443</t>
   </si>
   <si>
-    <t>Running solo on HPC</t>
-  </si>
-  <si>
     <t>Running solo on HPC (only 1 model)</t>
   </si>
   <si>
@@ -9177,9 +9174,6 @@
     <t>Running on HPC (1 model)</t>
   </si>
   <si>
-    <t>Running on HPC (still running)</t>
-  </si>
-  <si>
     <t>Running on HPC (only 1 model)</t>
   </si>
   <si>
@@ -9189,14 +9183,20 @@
     <t>Running on HPC (3 models)</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>1 model</t>
+  </si>
+  <si>
+    <t>0 models (RE-RUNNING)</t>
+  </si>
+  <si>
+    <t>0 models  (RE-RUNNING)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9429,6 +9429,12 @@
     <font>
       <u/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9901,7 +9907,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -10172,6 +10178,36 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10211,34 +10247,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -10639,28 +10648,28 @@
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
-      <c r="K1" s="110" t="s">
+      <c r="K1" s="120" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="113" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="123" t="s">
         <v>560</v>
       </c>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="104" t="s">
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="114" t="s">
         <v>561</v>
       </c>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="106"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="116"/>
       <c r="AC1" s="39" t="s">
         <v>2878</v>
       </c>
@@ -10676,16 +10685,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="38"/>
-      <c r="E2" s="108" t="s">
+      <c r="E2" s="118" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="107"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="107" t="s">
+      <c r="F2" s="117"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="117" t="s">
         <v>203</v>
       </c>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
       <c r="K2" s="8" t="s">
         <v>206</v>
       </c>
@@ -14908,9 +14917,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091D803E-5FC9-4756-B9B7-361382611093}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14977,7 +14986,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="106" t="s">
         <v>568</v>
       </c>
       <c r="C2" s="51">
@@ -14995,10 +15004,10 @@
       <c r="G2" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H2" s="125" t="s">
+      <c r="H2" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I2" s="125" t="s">
+      <c r="I2" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J2" s="63" t="s">
@@ -15014,7 +15023,7 @@
       <c r="N2" s="47"/>
     </row>
     <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="106" t="s">
         <v>569</v>
       </c>
       <c r="B3" s="87"/>
@@ -15033,10 +15042,10 @@
       <c r="G3" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H3" s="125" t="s">
+      <c r="H3" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I3" s="125" t="s">
+      <c r="I3" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J3" s="63" t="s">
@@ -15052,7 +15061,7 @@
       <c r="N3" s="47"/>
     </row>
     <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="106" t="s">
         <v>570</v>
       </c>
       <c r="C4" s="51">
@@ -15070,10 +15079,10 @@
       <c r="G4" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H4" s="61" t="s">
-        <v>2988</v>
-      </c>
-      <c r="I4" s="125" t="s">
+      <c r="H4" s="112" t="s">
+        <v>3026</v>
+      </c>
+      <c r="I4" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J4" s="63" t="s">
@@ -15089,7 +15098,7 @@
       <c r="N4" s="47"/>
     </row>
     <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="107" t="s">
         <v>2909</v>
       </c>
       <c r="C5" s="51">
@@ -15108,7 +15117,7 @@
         <v>2889</v>
       </c>
       <c r="H5" s="61" t="s">
-        <v>2988</v>
+        <v>3036</v>
       </c>
       <c r="I5" s="61" t="s">
         <v>3036</v>
@@ -15126,7 +15135,7 @@
       <c r="N5" s="47"/>
     </row>
     <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="106" t="s">
         <v>572</v>
       </c>
       <c r="C6" s="51">
@@ -15144,10 +15153,10 @@
       <c r="G6" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H6" s="125" t="s">
+      <c r="H6" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I6" s="125" t="s">
+      <c r="I6" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J6" s="63" t="s">
@@ -15163,7 +15172,7 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="119" t="s">
+      <c r="A7" s="106" t="s">
         <v>573</v>
       </c>
       <c r="C7" s="51">
@@ -15181,10 +15190,10 @@
       <c r="G7" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H7" s="125" t="s">
+      <c r="H7" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J7" s="63" t="s">
@@ -15200,7 +15209,7 @@
       <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="106" t="s">
         <v>575</v>
       </c>
       <c r="C8" s="51">
@@ -15218,10 +15227,10 @@
       <c r="G8" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H8" s="125" t="s">
+      <c r="H8" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I8" s="125" t="s">
+      <c r="I8" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J8" s="63" t="s">
@@ -15237,7 +15246,7 @@
       <c r="N8" s="47"/>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="106" t="s">
         <v>574</v>
       </c>
       <c r="C9" s="51">
@@ -15255,10 +15264,10 @@
       <c r="G9" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H9" s="125" t="s">
+      <c r="H9" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J9" s="63" t="s">
@@ -15274,7 +15283,7 @@
       <c r="N9" s="47"/>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="107" t="s">
         <v>576</v>
       </c>
       <c r="C10" s="51">
@@ -15293,9 +15302,9 @@
         <v>2889</v>
       </c>
       <c r="H10" s="61" t="s">
-        <v>2988</v>
-      </c>
-      <c r="I10" s="125" t="s">
+        <v>3036</v>
+      </c>
+      <c r="I10" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J10" s="63" t="s">
@@ -15311,7 +15320,7 @@
       <c r="N10" s="47"/>
     </row>
     <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="107" t="s">
         <v>577</v>
       </c>
       <c r="C11" s="51">
@@ -15330,10 +15339,10 @@
         <v>2889</v>
       </c>
       <c r="H11" s="61" t="s">
-        <v>2988</v>
+        <v>3034</v>
       </c>
       <c r="I11" s="61" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
       <c r="J11" s="63" t="s">
         <v>2916</v>
@@ -15348,7 +15357,7 @@
       <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="107" t="s">
         <v>578</v>
       </c>
       <c r="C12" s="51">
@@ -15367,7 +15376,7 @@
         <v>2889</v>
       </c>
       <c r="H12" s="61" t="s">
-        <v>2988</v>
+        <v>3034</v>
       </c>
       <c r="I12" s="61" t="s">
         <v>3036</v>
@@ -15385,7 +15394,7 @@
       <c r="N12" s="47"/>
     </row>
     <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="120" t="s">
+      <c r="A13" s="107" t="s">
         <v>579</v>
       </c>
       <c r="B13" s="87"/>
@@ -15405,9 +15414,9 @@
         <v>2889</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>2988</v>
-      </c>
-      <c r="I13" s="125" t="s">
+        <v>3036</v>
+      </c>
+      <c r="I13" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J13" s="63" t="s">
@@ -15423,7 +15432,7 @@
       <c r="N13" s="47"/>
     </row>
     <row r="14" spans="1:14" s="50" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="111" t="s">
         <v>580</v>
       </c>
       <c r="B14" s="88"/>
@@ -15443,9 +15452,9 @@
         <v>2889</v>
       </c>
       <c r="H14" s="62" t="s">
-        <v>2988</v>
-      </c>
-      <c r="I14" s="126" t="s">
+        <v>3036</v>
+      </c>
+      <c r="I14" s="113" t="s">
         <v>3026</v>
       </c>
       <c r="J14" s="64" t="s">
@@ -15461,7 +15470,7 @@
       <c r="N14" s="49"/>
     </row>
     <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="120" t="s">
+      <c r="A15" s="107" t="s">
         <v>2902</v>
       </c>
       <c r="C15" s="51">
@@ -15480,7 +15489,7 @@
         <v>2889</v>
       </c>
       <c r="H15" s="61" t="s">
-        <v>2988</v>
+        <v>3036</v>
       </c>
       <c r="I15" s="61" t="s">
         <v>3036</v>
@@ -15496,7 +15505,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="120" t="s">
+      <c r="A16" s="107" t="s">
         <v>2903</v>
       </c>
       <c r="C16" s="51">
@@ -15515,10 +15524,10 @@
         <v>2889</v>
       </c>
       <c r="H16" s="61" t="s">
-        <v>2988</v>
+        <v>3036</v>
       </c>
       <c r="I16" s="61" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
       <c r="J16" s="63" t="s">
         <v>2921</v>
@@ -15531,7 +15540,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="119" t="s">
+      <c r="A17" s="106" t="s">
         <v>2895</v>
       </c>
       <c r="C17" s="51">
@@ -15549,10 +15558,10 @@
       <c r="G17" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H17" s="125" t="s">
+      <c r="H17" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I17" s="125" t="s">
+      <c r="I17" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J17" s="63" t="s">
@@ -15566,7 +15575,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="119" t="s">
+      <c r="A18" s="106" t="s">
         <v>2896</v>
       </c>
       <c r="C18" s="51">
@@ -15584,10 +15593,10 @@
       <c r="G18" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H18" s="125" t="s">
+      <c r="H18" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I18" s="125" t="s">
+      <c r="I18" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J18" s="63" t="s">
@@ -15637,7 +15646,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="119" t="s">
+      <c r="A20" s="106" t="s">
         <v>2899</v>
       </c>
       <c r="C20" s="51">
@@ -15655,10 +15664,10 @@
       <c r="G20" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H20" s="125" t="s">
+      <c r="H20" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I20" s="125" t="s">
+      <c r="I20" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J20" s="63" t="s">
@@ -15672,7 +15681,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="120" t="s">
+      <c r="A21" s="107" t="s">
         <v>2900</v>
       </c>
       <c r="C21" s="51">
@@ -15690,7 +15699,7 @@
       <c r="G21" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H21" s="125" t="s">
+      <c r="H21" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="I21" s="61" t="s">
@@ -15707,7 +15716,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="106" t="s">
         <v>2901</v>
       </c>
       <c r="C22" s="51">
@@ -15725,10 +15734,10 @@
       <c r="G22" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H22" s="125" t="s">
+      <c r="H22" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I22" s="125" t="s">
+      <c r="I22" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J22" s="63" t="s">
@@ -15742,7 +15751,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="120" t="s">
+      <c r="A23" s="107" t="s">
         <v>2897</v>
       </c>
       <c r="C23" s="51">
@@ -15761,9 +15770,9 @@
         <v>2889</v>
       </c>
       <c r="H23" s="61" t="s">
-        <v>2988</v>
-      </c>
-      <c r="I23" s="125" t="s">
+        <v>3036</v>
+      </c>
+      <c r="I23" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J23" s="63" t="s">
@@ -15777,7 +15786,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" s="50" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="111" t="s">
         <v>2905</v>
       </c>
       <c r="B24" s="88"/>
@@ -15797,7 +15806,7 @@
         <v>2889</v>
       </c>
       <c r="H24" s="62" t="s">
-        <v>2988</v>
+        <v>3036</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>3036</v>
@@ -15813,7 +15822,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="120" t="s">
+      <c r="A25" s="107" t="s">
         <v>585</v>
       </c>
       <c r="C25" s="51">
@@ -15831,11 +15840,11 @@
       <c r="G25" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H25" s="117" t="s">
-        <v>3029</v>
-      </c>
-      <c r="I25" s="117" t="s">
-        <v>3033</v>
+      <c r="H25" s="104" t="s">
+        <v>3028</v>
+      </c>
+      <c r="I25" s="104" t="s">
+        <v>3031</v>
       </c>
       <c r="J25" s="65" t="s">
         <v>2990</v>
@@ -15848,7 +15857,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="119" t="s">
+      <c r="A26" s="106" t="s">
         <v>586</v>
       </c>
       <c r="C26" s="51">
@@ -15866,10 +15875,10 @@
       <c r="G26" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H26" s="125" t="s">
+      <c r="H26" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I26" s="125" t="s">
+      <c r="I26" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J26" s="65" t="s">
@@ -15883,7 +15892,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="106" t="s">
         <v>587</v>
       </c>
       <c r="C27" s="51">
@@ -15901,11 +15910,11 @@
       <c r="G27" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H27" s="125" t="s">
+      <c r="H27" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I27" s="117" t="s">
-        <v>3032</v>
+      <c r="I27" s="112" t="s">
+        <v>3026</v>
       </c>
       <c r="J27" s="65" t="s">
         <v>2992</v>
@@ -15918,7 +15927,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="106" t="s">
         <v>588</v>
       </c>
       <c r="C28" s="51">
@@ -15936,10 +15945,10 @@
       <c r="G28" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H28" s="125" t="s">
+      <c r="H28" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I28" s="125" t="s">
+      <c r="I28" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J28" s="65" t="s">
@@ -15953,7 +15962,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="119" t="s">
+      <c r="A29" s="106" t="s">
         <v>589</v>
       </c>
       <c r="C29" s="51">
@@ -15971,10 +15980,10 @@
       <c r="G29" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H29" s="125" t="s">
+      <c r="H29" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I29" s="125" t="s">
+      <c r="I29" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J29" s="65" t="s">
@@ -15988,7 +15997,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="106" t="s">
         <v>590</v>
       </c>
       <c r="C30" s="51">
@@ -16006,10 +16015,10 @@
       <c r="G30" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H30" s="125" t="s">
+      <c r="H30" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I30" s="125" t="s">
+      <c r="I30" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J30" s="65" t="s">
@@ -16023,7 +16032,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="119" t="s">
+      <c r="A31" s="106" t="s">
         <v>591</v>
       </c>
       <c r="C31" s="51">
@@ -16041,10 +16050,10 @@
       <c r="G31" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H31" s="125" t="s">
+      <c r="H31" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I31" s="125" t="s">
+      <c r="I31" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J31" s="65" t="s">
@@ -16058,7 +16067,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="119" t="s">
+      <c r="A32" s="106" t="s">
         <v>592</v>
       </c>
       <c r="C32" s="51">
@@ -16076,10 +16085,10 @@
       <c r="G32" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H32" s="125" t="s">
+      <c r="H32" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I32" s="125" t="s">
+      <c r="I32" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J32" s="65" t="s">
@@ -16093,7 +16102,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="119" t="s">
+      <c r="A33" s="106" t="s">
         <v>593</v>
       </c>
       <c r="C33" s="51">
@@ -16111,10 +16120,10 @@
       <c r="G33" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H33" s="125" t="s">
+      <c r="H33" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I33" s="125" t="s">
+      <c r="I33" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J33" s="65" t="s">
@@ -16128,7 +16137,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="106" t="s">
         <v>594</v>
       </c>
       <c r="C34" s="51">
@@ -16146,10 +16155,10 @@
       <c r="G34" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H34" s="125" t="s">
+      <c r="H34" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I34" s="125" t="s">
+      <c r="I34" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J34" s="65" t="s">
@@ -16163,7 +16172,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="119" t="s">
+      <c r="A35" s="106" t="s">
         <v>595</v>
       </c>
       <c r="C35" s="51">
@@ -16181,10 +16190,10 @@
       <c r="G35" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H35" s="125" t="s">
+      <c r="H35" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I35" s="125" t="s">
+      <c r="I35" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J35" s="65" t="s">
@@ -16198,7 +16207,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" s="86" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="110" t="s">
         <v>597</v>
       </c>
       <c r="B36" s="90" t="s">
@@ -16219,10 +16228,10 @@
       <c r="G36" s="81" t="s">
         <v>2989</v>
       </c>
-      <c r="H36" s="118" t="s">
-        <v>3028</v>
-      </c>
-      <c r="I36" s="125" t="s">
+      <c r="H36" s="127" t="s">
+        <v>3035</v>
+      </c>
+      <c r="I36" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J36" s="84" t="s">
@@ -16236,7 +16245,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="120" t="s">
+      <c r="A37" s="107" t="s">
         <v>598</v>
       </c>
       <c r="B37" s="91"/>
@@ -16255,11 +16264,11 @@
       <c r="G37" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H37" s="117" t="s">
+      <c r="H37" s="104" t="s">
+        <v>3029</v>
+      </c>
+      <c r="I37" s="104" t="s">
         <v>3030</v>
-      </c>
-      <c r="I37" s="117" t="s">
-        <v>3031</v>
       </c>
       <c r="J37" s="65" t="s">
         <v>3002</v>
@@ -16272,7 +16281,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" s="103" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="121" t="s">
+      <c r="A38" s="108" t="s">
         <v>596</v>
       </c>
       <c r="B38" s="98" t="s">
@@ -16293,10 +16302,10 @@
       <c r="G38" s="85" t="s">
         <v>2889</v>
       </c>
-      <c r="H38" s="125" t="s">
+      <c r="H38" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I38" s="125" t="s">
+      <c r="I38" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J38" s="102" t="s">
@@ -16310,7 +16319,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="120" t="s">
+      <c r="A39" s="107" t="s">
         <v>599</v>
       </c>
       <c r="C39" s="51">
@@ -16328,11 +16337,11 @@
       <c r="G39" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H39" s="117" t="s">
+      <c r="H39" s="104" t="s">
+        <v>3029</v>
+      </c>
+      <c r="I39" s="104" t="s">
         <v>3030</v>
-      </c>
-      <c r="I39" s="117" t="s">
-        <v>3031</v>
       </c>
       <c r="J39" s="65" t="s">
         <v>3003</v>
@@ -16345,7 +16354,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" s="50" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="122" t="s">
+      <c r="A40" s="109" t="s">
         <v>600</v>
       </c>
       <c r="B40" s="88"/>
@@ -16364,10 +16373,10 @@
       <c r="G40" s="55" t="s">
         <v>2889</v>
       </c>
-      <c r="H40" s="126" t="s">
+      <c r="H40" s="113" t="s">
         <v>3026</v>
       </c>
-      <c r="I40" s="126" t="s">
+      <c r="I40" s="113" t="s">
         <v>3026</v>
       </c>
       <c r="J40" s="66" t="s">
@@ -16381,7 +16390,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="119" t="s">
+      <c r="A41" s="106" t="s">
         <v>159</v>
       </c>
       <c r="C41" s="51">
@@ -16399,10 +16408,10 @@
       <c r="G41" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H41" s="125" t="s">
+      <c r="H41" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I41" s="125" t="s">
+      <c r="I41" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J41" s="65" t="s">
@@ -16416,7 +16425,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="106" t="s">
         <v>125</v>
       </c>
       <c r="C42" s="51">
@@ -16434,10 +16443,10 @@
       <c r="G42" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H42" s="125" t="s">
+      <c r="H42" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I42" s="125" t="s">
+      <c r="I42" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J42" s="65" t="s">
@@ -16451,7 +16460,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="119" t="s">
+      <c r="A43" s="106" t="s">
         <v>101</v>
       </c>
       <c r="C43" s="51">
@@ -16469,10 +16478,10 @@
       <c r="G43" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H43" s="125" t="s">
+      <c r="H43" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I43" s="125" t="s">
+      <c r="I43" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J43" s="65" t="s">
@@ -16486,7 +16495,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="107" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="51">
@@ -16504,11 +16513,11 @@
       <c r="G44" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H44" s="118" t="s">
-        <v>3034</v>
-      </c>
-      <c r="I44" s="118" t="s">
-        <v>3034</v>
+      <c r="H44" s="105" t="s">
+        <v>3032</v>
+      </c>
+      <c r="I44" s="105" t="s">
+        <v>3032</v>
       </c>
       <c r="J44" s="65" t="s">
         <v>3008</v>
@@ -16521,7 +16530,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="119" t="s">
+      <c r="A45" s="106" t="s">
         <v>102</v>
       </c>
       <c r="C45" s="51">
@@ -16539,10 +16548,10 @@
       <c r="G45" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H45" s="125" t="s">
+      <c r="H45" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I45" s="125" t="s">
+      <c r="I45" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J45" s="65" t="s">
@@ -16556,7 +16565,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="119" t="s">
+      <c r="A46" s="106" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="51">
@@ -16574,10 +16583,10 @@
       <c r="G46" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H46" s="125" t="s">
+      <c r="H46" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I46" s="125" t="s">
+      <c r="I46" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J46" s="65" t="s">
@@ -16591,7 +16600,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="119" t="s">
+      <c r="A47" s="106" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="51">
@@ -16609,10 +16618,10 @@
       <c r="G47" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H47" s="125" t="s">
+      <c r="H47" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I47" s="125" t="s">
+      <c r="I47" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J47" s="65" t="s">
@@ -16626,7 +16635,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" s="86" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="123" t="s">
+      <c r="A48" s="110" t="s">
         <v>160</v>
       </c>
       <c r="B48" s="90" t="s">
@@ -16647,11 +16656,11 @@
       <c r="G48" s="81" t="s">
         <v>2989</v>
       </c>
-      <c r="H48" s="118" t="s">
-        <v>3034</v>
-      </c>
-      <c r="I48" s="118" t="s">
-        <v>3034</v>
+      <c r="H48" s="105" t="s">
+        <v>3032</v>
+      </c>
+      <c r="I48" s="105" t="s">
+        <v>3032</v>
       </c>
       <c r="J48" s="84" t="s">
         <v>3012</v>
@@ -16664,7 +16673,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="120" t="s">
+      <c r="A49" s="107" t="s">
         <v>147</v>
       </c>
       <c r="C49" s="51">
@@ -16682,11 +16691,11 @@
       <c r="G49" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H49" s="118" t="s">
-        <v>3035</v>
-      </c>
-      <c r="I49" s="118" t="s">
-        <v>3035</v>
+      <c r="H49" s="105" t="s">
+        <v>3033</v>
+      </c>
+      <c r="I49" s="105" t="s">
+        <v>3033</v>
       </c>
       <c r="J49" s="65" t="s">
         <v>3013</v>
@@ -16699,7 +16708,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="119" t="s">
+      <c r="A50" s="106" t="s">
         <v>148</v>
       </c>
       <c r="C50" s="51">
@@ -16717,10 +16726,10 @@
       <c r="G50" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H50" s="125" t="s">
+      <c r="H50" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I50" s="125" t="s">
+      <c r="I50" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J50" s="65" t="s">
@@ -16734,7 +16743,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="120" t="s">
+      <c r="A51" s="107" t="s">
         <v>161</v>
       </c>
       <c r="C51" s="51">
@@ -16752,11 +16761,11 @@
       <c r="G51" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H51" s="118" t="s">
-        <v>3034</v>
-      </c>
-      <c r="I51" s="118" t="s">
-        <v>3034</v>
+      <c r="H51" s="105" t="s">
+        <v>3032</v>
+      </c>
+      <c r="I51" s="105" t="s">
+        <v>3032</v>
       </c>
       <c r="J51" s="65" t="s">
         <v>3015</v>
@@ -16769,7 +16778,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="119" t="s">
+      <c r="A52" s="106" t="s">
         <v>128</v>
       </c>
       <c r="C52" s="51">
@@ -16787,10 +16796,10 @@
       <c r="G52" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H52" s="125" t="s">
+      <c r="H52" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I52" s="125" t="s">
+      <c r="I52" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J52" s="65" t="s">
@@ -16804,7 +16813,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="119" t="s">
+      <c r="A53" s="106" t="s">
         <v>144</v>
       </c>
       <c r="C53" s="51">
@@ -16822,10 +16831,10 @@
       <c r="G53" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H53" s="125" t="s">
+      <c r="H53" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I53" s="125" t="s">
+      <c r="I53" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J53" s="65" t="s">
@@ -16839,7 +16848,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="119" t="s">
+      <c r="A54" s="106" t="s">
         <v>145</v>
       </c>
       <c r="C54" s="51">
@@ -16857,10 +16866,10 @@
       <c r="G54" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H54" s="125" t="s">
+      <c r="H54" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I54" s="125" t="s">
+      <c r="I54" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J54" s="65" t="s">
@@ -16874,7 +16883,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="119" t="s">
+      <c r="A55" s="106" t="s">
         <v>131</v>
       </c>
       <c r="C55" s="51">
@@ -16892,10 +16901,10 @@
       <c r="G55" s="54" t="s">
         <v>2889</v>
       </c>
-      <c r="H55" s="125" t="s">
+      <c r="H55" s="112" t="s">
         <v>3026</v>
       </c>
-      <c r="I55" s="125" t="s">
+      <c r="I55" s="112" t="s">
         <v>3026</v>
       </c>
       <c r="J55" s="65" t="s">
@@ -16936,6 +16945,7 @@
       <c r="J64" s="52"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="31" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{8DDBEB67-B1CB-4609-AF34-A3F0E54D7216}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{CDC80E01-8B88-4303-9A44-2448CE8C37C2}"/>
@@ -17017,16 +17027,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">

</xml_diff>